<commit_message>
added more precision to rotor measurements
</commit_message>
<xml_diff>
--- a/Testing/RotorTest/RotorTest.xlsx
+++ b/Testing/RotorTest/RotorTest.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbell44/Workspace/QCS/Testing/RotorTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26604CE-D5AD-5348-862F-B2AA826B34A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BF80E4-00E9-CD4C-99AF-F2739D98CD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9C060CD3-611B-8B4A-850C-C32BBA57694F}"/>
+    <workbookView xWindow="-33620" yWindow="10080" windowWidth="38400" windowHeight="23500" xr2:uid="{9C060CD3-611B-8B4A-850C-C32BBA57694F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Mass" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -259,7 +259,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -764,7 +764,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1312,7 +1312,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1817,7 +1817,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -2350,7 +2350,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -6063,7 +6063,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6101,7 +6101,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D2">
-        <f>C2*9.81</f>
+        <f t="shared" ref="D2:D9" si="0">C2*9.81</f>
         <v>0.20601000000000003</v>
       </c>
       <c r="E2">
@@ -6117,15 +6117,15 @@
         <v>89</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">B3/1000</f>
+        <f t="shared" ref="C3:C9" si="1">B3/1000</f>
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="D3">
-        <f>C3*9.81</f>
+        <f t="shared" si="0"/>
         <v>0.87309000000000003</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="1">D3*4</f>
+        <f t="shared" ref="E3:E9" si="2">D3*4</f>
         <v>3.4923600000000001</v>
       </c>
     </row>
@@ -6137,15 +6137,15 @@
         <v>191</v>
       </c>
       <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.191</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.191</v>
-      </c>
-      <c r="D4">
-        <f>C4*9.81</f>
         <v>1.8737100000000002</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4948400000000008</v>
       </c>
     </row>
@@ -6157,15 +6157,15 @@
         <v>329</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="D5">
-        <f>C5*9.81</f>
         <v>3.2274900000000004</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.909960000000002</v>
       </c>
     </row>
@@ -6177,15 +6177,15 @@
         <v>456</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="D6">
-        <f>C6*9.81</f>
         <v>4.4733600000000004</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.893440000000002</v>
       </c>
     </row>
@@ -6197,15 +6197,15 @@
         <v>593</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="D7">
-        <f>C7*9.81</f>
         <v>5.8173300000000001</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23.26932</v>
       </c>
     </row>
@@ -6217,15 +6217,15 @@
         <v>745</v>
       </c>
       <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.745</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.745</v>
-      </c>
-      <c r="D8">
-        <f>C8*9.81</f>
         <v>7.3084500000000006</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.233800000000002</v>
       </c>
     </row>
@@ -6237,15 +6237,15 @@
         <v>860</v>
       </c>
       <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.86</v>
-      </c>
-      <c r="D9">
-        <f>C9*9.81</f>
         <v>8.4366000000000003</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.746400000000001</v>
       </c>
     </row>
@@ -6277,15 +6277,15 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <f>B13/1000</f>
+        <f t="shared" ref="C13:C18" si="3">B13/1000</f>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D13">
-        <f>C13*9.81</f>
+        <f t="shared" ref="D13:D18" si="4">C13*9.81</f>
         <v>2.9430000000000001E-2</v>
       </c>
       <c r="E13">
-        <f>D13*$G$13</f>
+        <f t="shared" ref="E13:E18" si="5">D13*$G$13</f>
         <v>3.8259000000000001E-3</v>
       </c>
       <c r="G13">
@@ -6300,15 +6300,15 @@
         <v>7.5</v>
       </c>
       <c r="C14">
-        <f>B14/1000</f>
+        <f t="shared" si="3"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="D14">
-        <f>C14*9.81</f>
+        <f t="shared" si="4"/>
         <v>7.3575000000000002E-2</v>
       </c>
       <c r="E14">
-        <f>D14*$G$13</f>
+        <f t="shared" si="5"/>
         <v>9.5647500000000003E-3</v>
       </c>
     </row>
@@ -6320,15 +6320,15 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <f>B15/1000</f>
+        <f t="shared" si="3"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D15">
-        <f>C15*9.81</f>
+        <f t="shared" si="4"/>
         <v>0.14715</v>
       </c>
       <c r="E15">
-        <f>D15*$G$13</f>
+        <f t="shared" si="5"/>
         <v>1.9129500000000001E-2</v>
       </c>
     </row>
@@ -6340,15 +6340,15 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <f>B16/1000</f>
+        <f t="shared" si="3"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="D16">
-        <f>C16*9.81</f>
+        <f t="shared" si="4"/>
         <v>0.25506000000000001</v>
       </c>
       <c r="E16">
-        <f>D16*$G$13</f>
+        <f t="shared" si="5"/>
         <v>3.3157800000000001E-2</v>
       </c>
     </row>
@@ -6360,15 +6360,15 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <f>B17/1000</f>
+        <f t="shared" si="3"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D17">
-        <f>C17*9.81</f>
+        <f t="shared" si="4"/>
         <v>0.34335000000000004</v>
       </c>
       <c r="E17">
-        <f>D17*$G$13</f>
+        <f t="shared" si="5"/>
         <v>4.4635500000000009E-2</v>
       </c>
     </row>
@@ -6380,15 +6380,15 @@
         <v>50</v>
       </c>
       <c r="C18">
-        <f>B18/1000</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="D18">
-        <f>C18*9.81</f>
+        <f t="shared" si="4"/>
         <v>0.49050000000000005</v>
       </c>
       <c r="E18">
-        <f>D18*$G$13</f>
+        <f t="shared" si="5"/>
         <v>6.3765000000000002E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tunable parameters for control
</commit_message>
<xml_diff>
--- a/Testing/RotorTest/RotorTest.xlsx
+++ b/Testing/RotorTest/RotorTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbell44/Workspace/QCS/Testing/RotorTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BF80E4-00E9-CD4C-99AF-F2739D98CD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F346DD9-ABAF-9142-9BF4-E74F39C8F399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="10080" windowWidth="38400" windowHeight="23500" xr2:uid="{9C060CD3-611B-8B4A-850C-C32BBA57694F}"/>
+    <workbookView xWindow="-36740" yWindow="940" windowWidth="33600" windowHeight="20500" xr2:uid="{9C060CD3-611B-8B4A-850C-C32BBA57694F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>F (g)</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Throttle</t>
+  </si>
+  <si>
+    <t>motors</t>
+  </si>
+  <si>
+    <t>frame</t>
   </si>
 </sst>
 </file>
@@ -765,6 +771,56 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.0544579806722304E-2"/>
+                  <c:y val="0.28618598682660484"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -6062,8 +6118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69A29D-78E3-8247-B114-A181BB661913}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6400,10 +6456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD157714-268A-5B42-8C8A-899007F314BD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6463,6 +6519,30 @@
         <v>340</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <f>B12*4</f>
+        <v>144</v>
+      </c>
+      <c r="D12">
+        <f>C12+B13</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>